<commit_message>
Various fixes made to GHATIM (see log in workbook) and some to links
</commit_message>
<xml_diff>
--- a/CGE/2simulation.xlsx
+++ b/CGE/2simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\GHATIMGE\CGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8E0E22-0367-4322-A70F-A8BA7FD7C2CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C1E56F-CF97-4668-B014-C68404E36CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" firstSheet="2" activeTab="4" xr2:uid="{9A2D140B-014C-4B15-9877-381ABEF3DC74}"/>
   </bookViews>
@@ -7052,22 +7052,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D7:L7 C8:L70 R8:AA70">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:AA70">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AA70">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AA70">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7079,8 +7079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11:Z11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7520,34 +7520,34 @@
         <v>79</v>
       </c>
       <c r="Q11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="R11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="S11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="T11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="U11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="V11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="W11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="X11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="Y11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="Z11" s="13">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
@@ -7957,47 +7957,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N8:N14 D7:L7 Q8:Z16 C8:L14">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z16">
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:L15">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:L16">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:L16">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9345,7 +9345,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M8:M14 C7:K7 B8:K22 Q8:Z22">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29877,22 +29877,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D7 C9:C142 C8:AK8">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:BD7">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:AK142">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2 C2:L2 R2:AA2">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31545,8 +31545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6130A96-BF02-4FAE-B189-B2D054E8563F}">
   <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31850,7 +31850,7 @@
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
       <c r="O9">
-        <v>-0.3</v>
+        <v>-0.4</v>
       </c>
       <c r="P9" t="s">
         <v>222</v>
@@ -31860,31 +31860,31 @@
       </c>
       <c r="R9" s="16">
         <f>Q9+$O9</f>
-        <v>2.469729023435459</v>
+        <v>2.3697290234354589</v>
       </c>
       <c r="S9" s="16">
         <f t="shared" ref="S9:U9" si="5">R9+$O9</f>
-        <v>2.1697290234354591</v>
+        <v>1.969729023435459</v>
       </c>
       <c r="T9" s="16">
         <f t="shared" si="5"/>
-        <v>1.8697290234354591</v>
+        <v>1.5697290234354591</v>
       </c>
       <c r="U9" s="16">
         <f t="shared" si="5"/>
-        <v>1.5697290234354591</v>
+        <v>1.1697290234354591</v>
       </c>
       <c r="V9" s="16">
         <f t="shared" ref="V9:X9" si="6">U9+$O9</f>
-        <v>1.269729023435459</v>
+        <v>0.76972902343545913</v>
       </c>
       <c r="W9" s="16">
         <f t="shared" si="6"/>
-        <v>0.96972902343545897</v>
+        <v>0.3697290234354591</v>
       </c>
       <c r="X9" s="16">
         <f t="shared" si="6"/>
-        <v>0.66972902343545893</v>
+        <v>-3.0270976564540919E-2</v>
       </c>
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
@@ -32571,31 +32571,31 @@
         <v>3.1664804701843869</v>
       </c>
       <c r="R17" s="16">
-        <f>Q17+$O16</f>
+        <f t="shared" ref="R17:X19" si="26">Q17+$O16</f>
         <v>3.1664804701843869</v>
       </c>
       <c r="S17" s="16">
-        <f>R17+$O16</f>
+        <f t="shared" si="26"/>
         <v>3.1664804701843869</v>
       </c>
       <c r="T17" s="16">
-        <f>S17+$O16</f>
+        <f t="shared" si="26"/>
         <v>3.1664804701843869</v>
       </c>
       <c r="U17" s="16">
-        <f>T17+$O16</f>
+        <f t="shared" si="26"/>
         <v>3.1664804701843869</v>
       </c>
       <c r="V17" s="16">
-        <f>U17+$O16</f>
+        <f t="shared" si="26"/>
         <v>3.1664804701843869</v>
       </c>
       <c r="W17" s="16">
-        <f>V17+$O16</f>
+        <f t="shared" si="26"/>
         <v>3.1664804701843869</v>
       </c>
       <c r="X17" s="16">
-        <f>W17+$O16</f>
+        <f t="shared" si="26"/>
         <v>3.1664804701843869</v>
       </c>
       <c r="Y17" s="13"/>
@@ -32660,31 +32660,31 @@
         <v>0.34343701645363039</v>
       </c>
       <c r="R18" s="16">
-        <f>Q18+$O17</f>
+        <f t="shared" si="26"/>
         <v>0.34343701645363039</v>
       </c>
       <c r="S18" s="16">
-        <f>R18+$O17</f>
+        <f t="shared" si="26"/>
         <v>0.34343701645363039</v>
       </c>
       <c r="T18" s="16">
-        <f>S18+$O17</f>
+        <f t="shared" si="26"/>
         <v>0.34343701645363039</v>
       </c>
       <c r="U18" s="16">
-        <f>T18+$O17</f>
+        <f t="shared" si="26"/>
         <v>0.34343701645363039</v>
       </c>
       <c r="V18" s="16">
-        <f>U18+$O17</f>
+        <f t="shared" si="26"/>
         <v>0.34343701645363039</v>
       </c>
       <c r="W18" s="16">
-        <f>V18+$O17</f>
+        <f t="shared" si="26"/>
         <v>0.34343701645363039</v>
       </c>
       <c r="X18" s="16">
-        <f>W18+$O17</f>
+        <f t="shared" si="26"/>
         <v>0.34343701645363039</v>
       </c>
       <c r="Y18" s="13"/>
@@ -32747,31 +32747,31 @@
         <v>1.7452416690008683</v>
       </c>
       <c r="R19" s="16">
-        <f>Q19+$O18</f>
+        <f t="shared" si="26"/>
         <v>1.7452416690008683</v>
       </c>
       <c r="S19" s="16">
-        <f>R19+$O18</f>
+        <f t="shared" si="26"/>
         <v>1.7452416690008683</v>
       </c>
       <c r="T19" s="16">
-        <f>S19+$O18</f>
+        <f t="shared" si="26"/>
         <v>1.7452416690008683</v>
       </c>
       <c r="U19" s="16">
-        <f>T19+$O18</f>
+        <f t="shared" si="26"/>
         <v>1.7452416690008683</v>
       </c>
       <c r="V19" s="16">
-        <f>U19+$O18</f>
+        <f t="shared" si="26"/>
         <v>1.7452416690008683</v>
       </c>
       <c r="W19" s="16">
-        <f>V19+$O18</f>
+        <f t="shared" si="26"/>
         <v>1.7452416690008683</v>
       </c>
       <c r="X19" s="16">
-        <f>W19+$O18</f>
+        <f t="shared" si="26"/>
         <v>1.7452416690008683</v>
       </c>
       <c r="Y19" s="13"/>
@@ -33342,27 +33342,27 @@
       </c>
       <c r="E29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.21697290234354594</v>
+        <v>-0.19697290234354592</v>
       </c>
       <c r="F29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.3088103164048213</v>
+        <v>1.0988103164048213</v>
       </c>
       <c r="G29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.2557832187483673</v>
+        <v>0.93578321874836734</v>
       </c>
       <c r="H29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.0157832187483673</v>
+        <v>0.61578321874836739</v>
       </c>
       <c r="I29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.7757832187483672</v>
+        <v>0.29578321874836727</v>
       </c>
       <c r="J29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.53578321874836721</v>
+        <v>-2.4216781251632735E-2</v>
       </c>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
@@ -33402,27 +33402,27 @@
       </c>
       <c r="E30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.21697290234354594</v>
+        <v>-0.19697290234354592</v>
       </c>
       <c r="F30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.3088103164048213</v>
+        <v>1.0988103164048213</v>
       </c>
       <c r="G30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.2557832187483673</v>
+        <v>0.93578321874836734</v>
       </c>
       <c r="H30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.0157832187483673</v>
+        <v>0.61578321874836739</v>
       </c>
       <c r="I30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.7757832187483672</v>
+        <v>0.29578321874836727</v>
       </c>
       <c r="J30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.53578321874836721</v>
+        <v>-2.4216781251632735E-2</v>
       </c>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
@@ -33462,27 +33462,27 @@
       </c>
       <c r="E31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.21697290234354594</v>
+        <v>-0.19697290234354592</v>
       </c>
       <c r="F31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.3088103164048213</v>
+        <v>1.0988103164048213</v>
       </c>
       <c r="G31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.2557832187483673</v>
+        <v>0.93578321874836734</v>
       </c>
       <c r="H31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.0157832187483673</v>
+        <v>0.61578321874836739</v>
       </c>
       <c r="I31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.7757832187483672</v>
+        <v>0.29578321874836727</v>
       </c>
       <c r="J31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.53578321874836721</v>
+        <v>-2.4216781251632735E-2</v>
       </c>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
@@ -35838,12 +35838,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19:X19">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19:X19">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40935,12 +40935,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8:C63 D7:L63 C10:L70 R8:AA70">
-    <cfRule type="cellIs" dxfId="52" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="12" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:AA70">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42022,42 +42022,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:K7 B8:K17 Q8:Z17 Q19:Z21 B19:K21">
-    <cfRule type="cellIs" dxfId="50" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="19" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z17">
-    <cfRule type="cellIs" dxfId="49" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z17">
-    <cfRule type="cellIs" dxfId="48" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z17">
-    <cfRule type="cellIs" dxfId="47" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:K18 Q18:Z18">
-    <cfRule type="cellIs" dxfId="46" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q18:Z18">
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18:Z18">
-    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18:Z18">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42936,62 +42936,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:K7 Q8:Z16 B8:K16">
-    <cfRule type="cellIs" dxfId="42" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z16">
-    <cfRule type="cellIs" dxfId="41" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="24" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="40" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="23" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="39" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="22" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="38" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="21" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="37" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="20" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17 B17:K17">
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17">
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43836,57 +43836,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:K7 Q8:Z13 B8:K16">
-    <cfRule type="cellIs" dxfId="30" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z13">
-    <cfRule type="cellIs" dxfId="29" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:Z16">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:Z16">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:K17">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
With labour constraint fixed in CGE
</commit_message>
<xml_diff>
--- a/CGE/2simulation.xlsx
+++ b/CGE/2simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\GHATIMGE\CGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C1E56F-CF97-4668-B014-C68404E36CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462DB41E-CD48-4465-B999-5BA964CA1CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" firstSheet="2" activeTab="4" xr2:uid="{9A2D140B-014C-4B15-9877-381ABEF3DC74}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3174" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3176" uniqueCount="235">
   <si>
     <t>GDX index</t>
   </si>
@@ -915,7 +915,317 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="134">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.34998626667073579"/>
@@ -7052,22 +7362,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D7:L7 C8:L70 R8:AA70">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:AA70">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AA70">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AA70">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7080,7 +7390,7 @@
   <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7232,44 +7542,44 @@
       <c r="B8" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="13">
-        <v>6.8</v>
-      </c>
-      <c r="D8" s="13">
+      <c r="C8" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="13" t="str">
         <f>$C8</f>
-        <v>6.8</v>
-      </c>
-      <c r="E8" s="13">
+        <v>eps</v>
+      </c>
+      <c r="E8" s="13" t="str">
         <f t="shared" ref="E8:L16" si="1">$C8</f>
-        <v>6.8</v>
-      </c>
-      <c r="F8" s="13">
+        <v>eps</v>
+      </c>
+      <c r="F8" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="G8" s="13">
+        <v>eps</v>
+      </c>
+      <c r="G8" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="H8" s="13">
+        <v>eps</v>
+      </c>
+      <c r="H8" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="I8" s="13">
+        <v>eps</v>
+      </c>
+      <c r="I8" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="J8" s="13">
+        <v>eps</v>
+      </c>
+      <c r="J8" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="K8" s="13">
+        <v>eps</v>
+      </c>
+      <c r="K8" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="L8" s="13">
+        <v>eps</v>
+      </c>
+      <c r="L8" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
+        <v>eps</v>
       </c>
       <c r="N8" s="13"/>
       <c r="P8" t="s">
@@ -7476,7 +7786,6 @@
         <v>79</v>
       </c>
       <c r="C11" s="13">
-        <f>C8</f>
         <v>6.8</v>
       </c>
       <c r="D11" s="13">
@@ -7557,45 +7866,44 @@
       <c r="B12" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="13">
-        <f>C11</f>
-        <v>6.8</v>
-      </c>
-      <c r="D12" s="13">
-        <f t="shared" si="2"/>
-        <v>6.8</v>
-      </c>
-      <c r="E12" s="13">
+      <c r="C12" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>eps</v>
+      </c>
+      <c r="E12" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="F12" s="13">
+        <v>eps</v>
+      </c>
+      <c r="F12" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="G12" s="13">
+        <v>eps</v>
+      </c>
+      <c r="G12" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="H12" s="13">
+        <v>eps</v>
+      </c>
+      <c r="H12" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="I12" s="13">
+        <v>eps</v>
+      </c>
+      <c r="I12" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="J12" s="13">
+        <v>eps</v>
+      </c>
+      <c r="J12" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="K12" s="13">
+        <v>eps</v>
+      </c>
+      <c r="K12" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="L12" s="13">
+        <v>eps</v>
+      </c>
+      <c r="L12" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
+        <v>eps</v>
       </c>
       <c r="N12" s="13"/>
       <c r="P12" t="s">
@@ -7801,45 +8109,45 @@
       <c r="B15" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="13" t="str">
         <f>C12</f>
-        <v>6.8</v>
-      </c>
-      <c r="D15" s="13">
-        <f t="shared" si="2"/>
-        <v>6.8</v>
-      </c>
-      <c r="E15" s="13">
+        <v>eps</v>
+      </c>
+      <c r="D15" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>eps</v>
+      </c>
+      <c r="E15" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="F15" s="13">
+        <v>eps</v>
+      </c>
+      <c r="F15" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="G15" s="13">
+        <v>eps</v>
+      </c>
+      <c r="G15" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="H15" s="13">
+        <v>eps</v>
+      </c>
+      <c r="H15" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="I15" s="13">
+        <v>eps</v>
+      </c>
+      <c r="I15" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="J15" s="13">
+        <v>eps</v>
+      </c>
+      <c r="J15" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="K15" s="13">
+        <v>eps</v>
+      </c>
+      <c r="K15" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="L15" s="13">
+        <v>eps</v>
+      </c>
+      <c r="L15" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>6.8</v>
+        <v>eps</v>
       </c>
       <c r="P15" t="s">
         <v>121</v>
@@ -7956,48 +8264,88 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="N8:N14 D7:L7 Q8:Z16 C8:L14">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+  <conditionalFormatting sqref="N8:N14 D7:L7 C8:L14 Q8:Z16">
+    <cfRule type="cellIs" dxfId="44" priority="22" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z16">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="15" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="14" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="13" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="12" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:L15">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:L16">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:L16">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
+      <formula>"eps"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
+      <formula>"eps"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
+      <formula>"eps"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
+      <formula>"eps"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+      <formula>"eps"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+      <formula>"eps"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+      <formula>"eps"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+      <formula>"eps"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9345,7 +9693,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M8:M14 C7:K7 B8:K22 Q8:Z22">
-    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9358,8 +9706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC07D98-4721-4023-A15B-0EB759FEDA84}">
   <dimension ref="A1:BD142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29877,22 +30225,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D7 C9:C142 C8:AK8">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:BD7">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:AK142">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2 C2:L2 R2:AA2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31545,8 +31893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6130A96-BF02-4FAE-B189-B2D054E8563F}">
   <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31578,28 +31926,56 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C2" s="20">
+        <v>1.6</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="20">
+        <v>0.7</v>
+      </c>
+      <c r="G2" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="H2" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="I2" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="J2" s="20">
+        <f>I2</f>
+        <v>0.8</v>
+      </c>
+    </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1.8</v>
+      </c>
       <c r="C3" s="20">
         <v>1.6</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="20">
-        <v>-0.1</v>
+        <f>E2*$B$3</f>
+        <v>0.18000000000000002</v>
       </c>
       <c r="F3" s="20">
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="20">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H3" s="20">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I3" s="20">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="J3" s="20">
-        <f>I3</f>
         <v>0.8</v>
       </c>
     </row>
@@ -31639,7 +32015,7 @@
         <v>base</v>
       </c>
       <c r="J6" s="8" t="str">
-        <f t="shared" ref="J6" si="1">I6</f>
+        <f t="shared" ref="J6:K6" si="1">I6</f>
         <v>base</v>
       </c>
       <c r="K6" s="8"/>
@@ -31672,7 +32048,7 @@
         <v>2040</v>
       </c>
       <c r="J7" s="8">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
@@ -31690,7 +32066,7 @@
         <v>2021</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7:X7" si="2">F7</f>
+        <f t="shared" ref="T7:Y7" si="2">F7</f>
         <v>2023</v>
       </c>
       <c r="U7">
@@ -31707,7 +32083,7 @@
       </c>
       <c r="X7">
         <f t="shared" si="2"/>
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
@@ -31737,23 +32113,23 @@
       </c>
       <c r="E8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -31785,7 +32161,7 @@
         <v>1.0232987128173923</v>
       </c>
       <c r="V8" s="16">
-        <f t="shared" ref="V8:X8" si="4">U8+$O8</f>
+        <f t="shared" ref="V8:Y8" si="4">U8+$O8</f>
         <v>1.0232987128173923</v>
       </c>
       <c r="W8" s="16">
@@ -31824,23 +32200,23 @@
       </c>
       <c r="E9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -31875,7 +32251,7 @@
         <v>1.1697290234354591</v>
       </c>
       <c r="V9" s="16">
-        <f t="shared" ref="V9:X9" si="6">U9+$O9</f>
+        <f t="shared" ref="V9:Y9" si="6">U9+$O9</f>
         <v>0.76972902343545913</v>
       </c>
       <c r="W9" s="16">
@@ -31916,23 +32292,23 @@
       </c>
       <c r="E10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -31967,7 +32343,7 @@
         <v>1.2789395129730821</v>
       </c>
       <c r="V10" s="16">
-        <f t="shared" ref="V10:X10" si="8">U10+$O10</f>
+        <f t="shared" ref="V10:Y10" si="8">U10+$O10</f>
         <v>1.478939512973082</v>
       </c>
       <c r="W10" s="16">
@@ -32008,23 +32384,23 @@
       </c>
       <c r="E11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32056,7 +32432,7 @@
         <v>1.1446620704770036</v>
       </c>
       <c r="V11" s="16">
-        <f t="shared" ref="V11:X11" si="10">U11+$O11</f>
+        <f t="shared" ref="V11:Y11" si="10">U11+$O11</f>
         <v>1.1446620704770036</v>
       </c>
       <c r="W11" s="16">
@@ -32094,23 +32470,23 @@
       </c>
       <c r="E12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32142,7 +32518,7 @@
         <v>1.1766661011545976</v>
       </c>
       <c r="V12" s="16">
-        <f t="shared" ref="V12:X12" si="12">U12+$O12</f>
+        <f t="shared" ref="V12:Y12" si="12">U12+$O12</f>
         <v>1.1766661011545976</v>
       </c>
       <c r="W12" s="16">
@@ -32180,23 +32556,23 @@
       </c>
       <c r="E13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32228,7 +32604,7 @@
         <v>1.0345883254866743</v>
       </c>
       <c r="V13" s="16">
-        <f t="shared" ref="V13:X13" si="14">U13+$O13</f>
+        <f t="shared" ref="V13:Y13" si="14">U13+$O13</f>
         <v>1.0345883254866743</v>
       </c>
       <c r="W13" s="16">
@@ -32269,23 +32645,23 @@
       </c>
       <c r="E14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32317,7 +32693,7 @@
         <v>1.4935970790688271</v>
       </c>
       <c r="V14" s="16">
-        <f t="shared" ref="V14:X14" si="16">U14+$O14</f>
+        <f t="shared" ref="V14:Y14" si="16">U14+$O14</f>
         <v>1.4935970790688271</v>
       </c>
       <c r="W14" s="16">
@@ -32358,23 +32734,23 @@
       </c>
       <c r="E15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32409,7 +32785,7 @@
         <v>1.2865935867004883</v>
       </c>
       <c r="V15" s="16">
-        <f t="shared" ref="V15:X15" si="18">U15+$O15</f>
+        <f t="shared" ref="V15:Y15" si="18">U15+$O15</f>
         <v>1.4865935867004882</v>
       </c>
       <c r="W15" s="16">
@@ -32450,23 +32826,23 @@
       </c>
       <c r="E16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32506,7 +32882,7 @@
         <v>1.4468415717265699</v>
       </c>
       <c r="X16" s="16">
-        <f t="shared" ref="X16" si="25">W16+$O16</f>
+        <f t="shared" ref="X16:Y16" si="25">W16+$O16</f>
         <v>1.4468415717265699</v>
       </c>
       <c r="Y16" s="13"/>
@@ -32539,23 +32915,23 @@
       </c>
       <c r="E17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32571,7 +32947,7 @@
         <v>3.1664804701843869</v>
       </c>
       <c r="R17" s="16">
-        <f t="shared" ref="R17:X19" si="26">Q17+$O16</f>
+        <f t="shared" ref="R17:Y19" si="26">Q17+$O16</f>
         <v>3.1664804701843869</v>
       </c>
       <c r="S17" s="16">
@@ -32628,23 +33004,23 @@
       </c>
       <c r="E18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32715,23 +33091,23 @@
       </c>
       <c r="E19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32802,23 +33178,23 @@
       </c>
       <c r="E20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32862,23 +33238,23 @@
       </c>
       <c r="E21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32922,23 +33298,23 @@
       </c>
       <c r="E22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -32982,23 +33358,23 @@
       </c>
       <c r="E23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33042,23 +33418,23 @@
       </c>
       <c r="E24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33102,23 +33478,23 @@
       </c>
       <c r="E25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33162,23 +33538,23 @@
       </c>
       <c r="E26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33222,23 +33598,23 @@
       </c>
       <c r="E27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33282,23 +33658,23 @@
       </c>
       <c r="E28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10232987128173923</v>
+        <v>0.18419376830713063</v>
       </c>
       <c r="F28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.71630909897217454</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="G28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="H28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.1256285840991316</v>
       </c>
       <c r="I28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.81863897025391386</v>
+        <v>0.92096884153565306</v>
       </c>
       <c r="J28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33342,23 +33718,23 @@
       </c>
       <c r="E29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.19697290234354592</v>
+        <v>0.35455122421838264</v>
       </c>
       <c r="F29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.0988103164048213</v>
+        <v>1.7267019257790051</v>
       </c>
       <c r="G29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.93578321874836734</v>
+        <v>1.2867019257790051</v>
       </c>
       <c r="H29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.61578321874836739</v>
+        <v>0.84670192577900516</v>
       </c>
       <c r="I29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.29578321874836727</v>
+        <v>0.33275612109191322</v>
       </c>
       <c r="J29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33402,23 +33778,23 @@
       </c>
       <c r="E30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.19697290234354592</v>
+        <v>0.35455122421838264</v>
       </c>
       <c r="F30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.0988103164048213</v>
+        <v>1.7267019257790051</v>
       </c>
       <c r="G30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.93578321874836734</v>
+        <v>1.2867019257790051</v>
       </c>
       <c r="H30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.61578321874836739</v>
+        <v>0.84670192577900516</v>
       </c>
       <c r="I30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.29578321874836727</v>
+        <v>0.33275612109191322</v>
       </c>
       <c r="J30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33462,23 +33838,23 @@
       </c>
       <c r="E31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.19697290234354592</v>
+        <v>0.35455122421838264</v>
       </c>
       <c r="F31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.0988103164048213</v>
+        <v>1.7267019257790051</v>
       </c>
       <c r="G31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.93578321874836734</v>
+        <v>1.2867019257790051</v>
       </c>
       <c r="H31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.61578321874836739</v>
+        <v>0.84670192577900516</v>
       </c>
       <c r="I31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.29578321874836727</v>
+        <v>0.33275612109191322</v>
       </c>
       <c r="J31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33522,23 +33898,23 @@
       </c>
       <c r="E32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33582,23 +33958,23 @@
       </c>
       <c r="E33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33642,23 +34018,23 @@
       </c>
       <c r="E34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33702,23 +34078,23 @@
       </c>
       <c r="E35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33762,23 +34138,23 @@
       </c>
       <c r="E36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33822,23 +34198,23 @@
       </c>
       <c r="E37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33882,23 +34258,23 @@
       </c>
       <c r="E38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -33942,23 +34318,23 @@
       </c>
       <c r="E39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34002,23 +34378,23 @@
       </c>
       <c r="E40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34062,23 +34438,23 @@
       </c>
       <c r="E41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34122,23 +34498,23 @@
       </c>
       <c r="E42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34182,23 +34558,23 @@
       </c>
       <c r="E43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34242,23 +34618,23 @@
       </c>
       <c r="E44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34302,23 +34678,23 @@
       </c>
       <c r="E45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34362,23 +34738,23 @@
       </c>
       <c r="E46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34422,23 +34798,23 @@
       </c>
       <c r="E47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34482,23 +34858,23 @@
       </c>
       <c r="E48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34542,23 +34918,23 @@
       </c>
       <c r="E49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.7893951297308218E-2</v>
+        <v>0.15820911233515481</v>
       </c>
       <c r="F49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.75525765908115738</v>
+        <v>1.1868334642703904</v>
       </c>
       <c r="G49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0231516103784657</v>
+        <v>1.4068334642703904</v>
       </c>
       <c r="H49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1831516103784656</v>
+        <v>1.6268334642703903</v>
       </c>
       <c r="I49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3431516103784658</v>
+        <v>1.5110455616757739</v>
       </c>
       <c r="J49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34654,23 +35030,23 @@
       </c>
       <c r="E51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.11446620704770037</v>
+        <v>0.20603917268586067</v>
       </c>
       <c r="F51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.80126344933390248</v>
+        <v>1.2591282775247041</v>
       </c>
       <c r="G51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.91572965638160297</v>
+        <v>1.2591282775247041</v>
       </c>
       <c r="H51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.91572965638160297</v>
+        <v>1.2591282775247041</v>
       </c>
       <c r="I51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.91572965638160297</v>
+        <v>1.0301958634293034</v>
       </c>
       <c r="J51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34714,23 +35090,23 @@
       </c>
       <c r="E52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.11766661011545976</v>
+        <v>0.21179989820782757</v>
       </c>
       <c r="F52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.8236662708082183</v>
+        <v>1.2943327112700573</v>
       </c>
       <c r="G52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.94133288092367806</v>
+        <v>1.2943327112700573</v>
       </c>
       <c r="H52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.94133288092367806</v>
+        <v>1.2943327112700573</v>
       </c>
       <c r="I52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.94133288092367806</v>
+        <v>1.0589994910391378</v>
       </c>
       <c r="J52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34774,23 +35150,23 @@
       </c>
       <c r="E53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10345883254866745</v>
+        <v>0.18622589858760141</v>
       </c>
       <c r="F53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.72421182784067195</v>
+        <v>1.138047158035342</v>
       </c>
       <c r="G53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.82767066038933956</v>
+        <v>1.138047158035342</v>
       </c>
       <c r="H53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.82767066038933956</v>
+        <v>1.138047158035342</v>
       </c>
       <c r="I53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.82767066038933956</v>
+        <v>0.93112949293800695</v>
       </c>
       <c r="J53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34834,23 +35210,23 @@
       </c>
       <c r="E54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.14935970790688272</v>
+        <v>0.26884747423238892</v>
       </c>
       <c r="F54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.0455179553481788</v>
+        <v>1.64295678697571</v>
       </c>
       <c r="G54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1948776632550617</v>
+        <v>1.64295678697571</v>
       </c>
       <c r="H54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1948776632550617</v>
+        <v>1.64295678697571</v>
       </c>
       <c r="I54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.1948776632550617</v>
+        <v>1.3442373711619444</v>
       </c>
       <c r="J54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34894,23 +35270,23 @@
       </c>
       <c r="E55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.10345883254866745</v>
+        <v>0.18622589858760141</v>
       </c>
       <c r="F55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.72421182784067195</v>
+        <v>1.138047158035342</v>
       </c>
       <c r="G55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.82767066038933956</v>
+        <v>1.138047158035342</v>
       </c>
       <c r="H55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.82767066038933956</v>
+        <v>1.138047158035342</v>
       </c>
       <c r="I55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.82767066038933956</v>
+        <v>0.93112949293800695</v>
       </c>
       <c r="J55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -34954,23 +35330,23 @@
       </c>
       <c r="E56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.14935970790688272</v>
+        <v>0.26884747423238892</v>
       </c>
       <c r="F56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.0455179553481788</v>
+        <v>1.64295678697571</v>
       </c>
       <c r="G56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1948776632550617</v>
+        <v>1.64295678697571</v>
       </c>
       <c r="H56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1948776632550617</v>
+        <v>1.64295678697571</v>
       </c>
       <c r="I56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.1948776632550617</v>
+        <v>1.3442373711619444</v>
       </c>
       <c r="J56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -35014,23 +35390,23 @@
       </c>
       <c r="E57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.14468415717265701</v>
+        <v>0.26043148291078261</v>
       </c>
       <c r="F57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.0127891002085989</v>
+        <v>1.5915257288992271</v>
       </c>
       <c r="G57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1574732573812561</v>
+        <v>1.5915257288992271</v>
       </c>
       <c r="H57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1574732573812561</v>
+        <v>1.5915257288992271</v>
       </c>
       <c r="I57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.1574732573812561</v>
+        <v>1.302157414553913</v>
       </c>
       <c r="J57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -35074,23 +35450,23 @@
       </c>
       <c r="E58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.31664804701843874</v>
+        <v>0.56996648463318966</v>
       </c>
       <c r="F58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>2.2165363291290707</v>
+        <v>3.4831285172028261</v>
       </c>
       <c r="G58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>2.5331843761475099</v>
+        <v>3.4831285172028261</v>
       </c>
       <c r="H58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>2.5331843761475099</v>
+        <v>3.4831285172028261</v>
       </c>
       <c r="I58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>2.5331843761475099</v>
+        <v>2.8498324231659482</v>
       </c>
       <c r="J58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -35134,23 +35510,23 @@
       </c>
       <c r="E59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-8.8659358670048843E-2</v>
+        <v>0.15958684560608793</v>
       </c>
       <c r="F59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.76061551069034183</v>
+        <v>1.1952529453705372</v>
       </c>
       <c r="G59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.0292748693603906</v>
+        <v>1.4152529453705371</v>
       </c>
       <c r="H59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1892748693603907</v>
+        <v>1.6352529453705371</v>
       </c>
       <c r="I59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3492748693603906</v>
+        <v>1.5179342280304393</v>
       </c>
       <c r="J59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -35194,23 +35570,23 @@
       </c>
       <c r="E60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-3.4343701645363038E-2</v>
+        <v>6.1818662961653476E-2</v>
       </c>
       <c r="F60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>0.24040591151754126</v>
+        <v>0.37778071809899344</v>
       </c>
       <c r="G60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.2747496131629043</v>
+        <v>0.37778071809899344</v>
       </c>
       <c r="H60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.2747496131629043</v>
+        <v>0.37778071809899344</v>
       </c>
       <c r="I60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.2747496131629043</v>
+        <v>0.30909331480826735</v>
       </c>
       <c r="J60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -35254,23 +35630,23 @@
       </c>
       <c r="E61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.17452416690008685</v>
+        <v>0.31414350042015632</v>
       </c>
       <c r="F61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.2216691683006078</v>
+        <v>1.9197658359009553</v>
       </c>
       <c r="G61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.3961933352006948</v>
+        <v>1.9197658359009553</v>
       </c>
       <c r="H61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.3961933352006948</v>
+        <v>1.9197658359009553</v>
       </c>
       <c r="I61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3961933352006948</v>
+        <v>1.5707175021007815</v>
       </c>
       <c r="J61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -35314,23 +35690,23 @@
       </c>
       <c r="E62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.17452416690008685</v>
+        <v>0.31414350042015632</v>
       </c>
       <c r="F62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.2216691683006078</v>
+        <v>1.9197658359009553</v>
       </c>
       <c r="G62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.3961933352006948</v>
+        <v>1.9197658359009553</v>
       </c>
       <c r="H62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.3961933352006948</v>
+        <v>1.9197658359009553</v>
       </c>
       <c r="I62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3961933352006948</v>
+        <v>1.5707175021007815</v>
       </c>
       <c r="J62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -35374,23 +35750,23 @@
       </c>
       <c r="E63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>-0.17452416690008685</v>
+        <v>0.31414350042015632</v>
       </c>
       <c r="F63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.2216691683006078</v>
+        <v>1.9197658359009553</v>
       </c>
       <c r="G63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.3961933352006948</v>
+        <v>1.9197658359009553</v>
       </c>
       <c r="H63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.3961933352006948</v>
+        <v>1.9197658359009553</v>
       </c>
       <c r="I63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3961933352006948</v>
+        <v>1.5707175021007815</v>
       </c>
       <c r="J63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
@@ -35588,262 +35964,262 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C55:C56 C64:E70 C59 C33:C50 C30:C31 C9:C28 C62:C63 H64:H70 J64:M70 K8:M63 S8:U8 S18:AB18 Y8:AB8 Y9:Z17 AB9:AB17 S17:X18 S10:X15 S20:AB70 Y19:AB19">
-    <cfRule type="cellIs" dxfId="102" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="65" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:U8 S18:AB18 Y8:AB8 Y9:Z17 AB9:AB17 S20:AB70 Y19:AB19">
-    <cfRule type="cellIs" dxfId="101" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="64" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64:I70">
-    <cfRule type="cellIs" dxfId="100" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="63" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G64:G70">
-    <cfRule type="cellIs" dxfId="99" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="62" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1">
-    <cfRule type="cellIs" dxfId="98" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="52" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:J63">
-    <cfRule type="cellIs" dxfId="97" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="51" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N1 R1 P1">
-    <cfRule type="cellIs" dxfId="96" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="57" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1">
-    <cfRule type="cellIs" dxfId="95" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="56" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="cellIs" dxfId="94" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="55" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1 Q1">
-    <cfRule type="cellIs" dxfId="93" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="54" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1">
-    <cfRule type="cellIs" dxfId="92" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="53" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="91" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="36" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="90" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="35" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E8 G8:J8">
-    <cfRule type="cellIs" dxfId="89" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="43" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="88" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="42" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="87" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="41" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8 I8">
-    <cfRule type="cellIs" dxfId="86" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="40" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="85" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="39" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="84" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="38" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="83" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="37" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53">
-    <cfRule type="cellIs" dxfId="82" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="34" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="81" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="33" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="cellIs" dxfId="80" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="32" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="79" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="31" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="78" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="30" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55:E56 D62:E63 D58:E59 D33:E50 D30:E31 D9:E28 G9:J28 G30:J31 G33:J50 G58:J59 G62:J63 G55:J56">
-    <cfRule type="cellIs" dxfId="77" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="29" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:E29 G29:J29">
-    <cfRule type="cellIs" dxfId="76" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="28" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:E32 G32:J32">
-    <cfRule type="cellIs" dxfId="75" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="27" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:E51 G51:J51">
-    <cfRule type="cellIs" dxfId="74" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="26" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:E53 G52:J53">
-    <cfRule type="cellIs" dxfId="73" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="25" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54:E54 G54:J54">
-    <cfRule type="cellIs" dxfId="72" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="24" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:E57 G57:J57">
-    <cfRule type="cellIs" dxfId="71" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="23" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60:E60 G60:J60">
-    <cfRule type="cellIs" dxfId="70" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="22" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61:E61 G61:J61">
-    <cfRule type="cellIs" dxfId="69" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="21" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64:F70">
-    <cfRule type="cellIs" dxfId="68" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="20" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="67" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="19" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="66" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="18" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55:F56 F62:F63 F58:F59 F33:F50 F30:F31 F9:F28">
-    <cfRule type="cellIs" dxfId="65" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="17" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="cellIs" dxfId="64" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="16" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="63" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="15" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="cellIs" dxfId="62" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="14" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:F53">
-    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="13" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="cellIs" dxfId="60" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="12" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="cellIs" dxfId="59" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60">
-    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61">
-    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V8:X8">
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V8:X8">
-    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16:X16">
-    <cfRule type="cellIs" dxfId="54" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19:X19">
-    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19:X19">
-    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40935,12 +41311,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8:C63 D7:L63 C10:L70 R8:AA70">
-    <cfRule type="cellIs" dxfId="50" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="12" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:AA70">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40952,7 +41328,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -42022,42 +42400,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:K7 B8:K17 Q8:Z17 Q19:Z21 B19:K21">
-    <cfRule type="cellIs" dxfId="48" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="19" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z17">
-    <cfRule type="cellIs" dxfId="47" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z17">
-    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z17">
-    <cfRule type="cellIs" dxfId="45" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:K18 Q18:Z18">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q18:Z18">
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18:Z18">
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18:Z18">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42069,7 +42447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -42215,43 +42595,43 @@
         <v>185</v>
       </c>
       <c r="B8" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C8" s="13">
         <f>B8</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D8" s="13">
         <f t="shared" ref="D8:K8" si="1">C8</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F8" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G8" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H8" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I8" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J8" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K8" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" ref="P8:P11" si="2">A8</f>
@@ -42293,43 +42673,43 @@
         <v>186</v>
       </c>
       <c r="B9" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C9" s="13">
         <f t="shared" ref="C9:K16" si="3">B9</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D9" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F9" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G9" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H9" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I9" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J9" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K9" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" si="2"/>
@@ -42371,43 +42751,43 @@
         <v>187</v>
       </c>
       <c r="B10" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C10" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D10" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H10" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I10" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J10" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K10" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="2"/>
@@ -42449,43 +42829,43 @@
         <v>188</v>
       </c>
       <c r="B11" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C11" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D11" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E11" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F11" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H11" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I11" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J11" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K11" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" si="2"/>
@@ -42527,43 +42907,43 @@
         <v>189</v>
       </c>
       <c r="B12" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C12" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D12" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E12" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F12" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G12" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H12" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I12" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J12" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K12" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" ref="P12:P16" si="4">A12</f>
@@ -42605,43 +42985,43 @@
         <v>190</v>
       </c>
       <c r="B13" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C13" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D13" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E13" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F13" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G13" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H13" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I13" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J13" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K13" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="4"/>
@@ -42683,43 +43063,43 @@
         <v>191</v>
       </c>
       <c r="B14" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C14" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D14" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E14" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F14" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G14" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H14" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I14" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J14" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K14" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" si="4"/>
@@ -42761,43 +43141,43 @@
         <v>192</v>
       </c>
       <c r="B15" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C15" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D15" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E15" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F15" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="G15" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H15" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="I15" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="J15" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K15" s="13">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="4"/>
@@ -42936,62 +43316,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:K7 Q8:Z16 B8:K16">
-    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="30" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z16">
-    <cfRule type="cellIs" dxfId="39" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="24" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="38" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="23" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="37" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="22" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="36" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="21" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="35" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="20" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17 B17:K17">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43836,57 +44216,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:K7 Q8:Z13 B8:K16">
-    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z13">
-    <cfRule type="cellIs" dxfId="27" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="25" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:Z16">
-    <cfRule type="cellIs" dxfId="22" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:Z16">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:K17">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
changes made for December runs + some updates on 1model.xls and 2simulat
</commit_message>
<xml_diff>
--- a/CGE/2simulation.xlsx
+++ b/CGE/2simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\GHATIMGE\CGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462DB41E-CD48-4465-B999-5BA964CA1CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CC403F-113C-4E7F-931A-F2A38DDD6817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" firstSheet="2" activeTab="4" xr2:uid="{9A2D140B-014C-4B15-9877-381ABEF3DC74}"/>
   </bookViews>
@@ -915,237 +915,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="134">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="111">
     <dxf>
       <font>
         <color theme="0" tint="-0.34998626667073579"/>
@@ -2850,7 +2620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -7362,22 +7134,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D7:L7 C8:L70 R8:AA70">
-    <cfRule type="cellIs" dxfId="48" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:AA70">
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AA70">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AA70">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8265,87 +8037,87 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N8:N14 D7:L7 C8:L14 Q8:Z16">
-    <cfRule type="cellIs" dxfId="44" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z16">
-    <cfRule type="cellIs" dxfId="43" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="42" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="41" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="40" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="39" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:L15">
-    <cfRule type="cellIs" dxfId="38" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:L16">
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:L16">
-    <cfRule type="cellIs" dxfId="36" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="cellIs" dxfId="30" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9693,7 +9465,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M8:M14 C7:K7 B8:K22 Q8:Z22">
-    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30225,22 +29997,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D7 C9:C142 C8:AK8">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:BD7">
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:AK142">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2 C2:L2 R2:AA2">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31054,7 +30826,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H18"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31893,8 +31665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6130A96-BF02-4FAE-B189-B2D054E8563F}">
   <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31903,6 +31675,9 @@
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="G1">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="L1" s="13">
         <v>2.7</v>
       </c>
@@ -31953,7 +31728,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B3">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="C3" s="20">
         <v>1.6</v>
@@ -31961,22 +31736,22 @@
       <c r="D3" s="20"/>
       <c r="E3" s="20">
         <f>E2*$B$3</f>
-        <v>0.18000000000000002</v>
+        <v>0.2</v>
       </c>
       <c r="F3" s="20">
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="20">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="H3" s="20">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="I3" s="20">
-        <v>0.9</v>
+        <v>1.2</v>
       </c>
       <c r="J3" s="20">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
@@ -32015,7 +31790,7 @@
         <v>base</v>
       </c>
       <c r="J6" s="8" t="str">
-        <f t="shared" ref="J6:K6" si="1">I6</f>
+        <f t="shared" ref="J6" si="1">I6</f>
         <v>base</v>
       </c>
       <c r="K6" s="8"/>
@@ -32066,7 +31841,7 @@
         <v>2021</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7:Y7" si="2">F7</f>
+        <f t="shared" ref="T7:X7" si="2">F7</f>
         <v>2023</v>
       </c>
       <c r="U7">
@@ -32113,7 +31888,7 @@
       </c>
       <c r="E8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32121,19 +31896,19 @@
       </c>
       <c r="G8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J8" s="13">
         <f>VLOOKUP(VLOOKUP($A8,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -32161,7 +31936,7 @@
         <v>1.0232987128173923</v>
       </c>
       <c r="V8" s="16">
-        <f t="shared" ref="V8:Y8" si="4">U8+$O8</f>
+        <f t="shared" ref="V8:X8" si="4">U8+$O8</f>
         <v>1.0232987128173923</v>
       </c>
       <c r="W8" s="16">
@@ -32200,7 +31975,7 @@
       </c>
       <c r="E9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32208,19 +31983,19 @@
       </c>
       <c r="G9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J9" s="13">
         <f>VLOOKUP(VLOOKUP($A9,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -32251,7 +32026,7 @@
         <v>1.1697290234354591</v>
       </c>
       <c r="V9" s="16">
-        <f t="shared" ref="V9:Y9" si="6">U9+$O9</f>
+        <f t="shared" ref="V9:X9" si="6">U9+$O9</f>
         <v>0.76972902343545913</v>
       </c>
       <c r="W9" s="16">
@@ -32292,7 +32067,7 @@
       </c>
       <c r="E10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32300,19 +32075,19 @@
       </c>
       <c r="G10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J10" s="13">
         <f>VLOOKUP(VLOOKUP($A10,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -32343,7 +32118,7 @@
         <v>1.2789395129730821</v>
       </c>
       <c r="V10" s="16">
-        <f t="shared" ref="V10:Y10" si="8">U10+$O10</f>
+        <f t="shared" ref="V10:X10" si="8">U10+$O10</f>
         <v>1.478939512973082</v>
       </c>
       <c r="W10" s="16">
@@ -32384,7 +32159,7 @@
       </c>
       <c r="E11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32392,19 +32167,19 @@
       </c>
       <c r="G11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J11" s="13">
         <f>VLOOKUP(VLOOKUP($A11,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -32432,7 +32207,7 @@
         <v>1.1446620704770036</v>
       </c>
       <c r="V11" s="16">
-        <f t="shared" ref="V11:Y11" si="10">U11+$O11</f>
+        <f t="shared" ref="V11:X11" si="10">U11+$O11</f>
         <v>1.1446620704770036</v>
       </c>
       <c r="W11" s="16">
@@ -32470,7 +32245,7 @@
       </c>
       <c r="E12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32478,19 +32253,19 @@
       </c>
       <c r="G12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J12" s="13">
         <f>VLOOKUP(VLOOKUP($A12,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -32518,7 +32293,7 @@
         <v>1.1766661011545976</v>
       </c>
       <c r="V12" s="16">
-        <f t="shared" ref="V12:Y12" si="12">U12+$O12</f>
+        <f t="shared" ref="V12:X12" si="12">U12+$O12</f>
         <v>1.1766661011545976</v>
       </c>
       <c r="W12" s="16">
@@ -32556,7 +32331,7 @@
       </c>
       <c r="E13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32564,19 +32339,19 @@
       </c>
       <c r="G13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J13" s="13">
         <f>VLOOKUP(VLOOKUP($A13,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -32604,7 +32379,7 @@
         <v>1.0345883254866743</v>
       </c>
       <c r="V13" s="16">
-        <f t="shared" ref="V13:Y13" si="14">U13+$O13</f>
+        <f t="shared" ref="V13:X13" si="14">U13+$O13</f>
         <v>1.0345883254866743</v>
       </c>
       <c r="W13" s="16">
@@ -32645,7 +32420,7 @@
       </c>
       <c r="E14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32653,23 +32428,26 @@
       </c>
       <c r="G14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J14" s="13">
         <f>VLOOKUP(VLOOKUP($A14,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
+      <c r="O14">
+        <v>0.1</v>
+      </c>
       <c r="P14" t="s">
         <v>230</v>
       </c>
@@ -32678,31 +32456,31 @@
       </c>
       <c r="R14" s="16">
         <f t="shared" ref="R14:U14" si="15">Q14+$O14</f>
-        <v>1.4935970790688271</v>
+        <v>1.5935970790688272</v>
       </c>
       <c r="S14" s="16">
         <f t="shared" si="15"/>
-        <v>1.4935970790688271</v>
+        <v>1.6935970790688273</v>
       </c>
       <c r="T14" s="16">
         <f t="shared" si="15"/>
-        <v>1.4935970790688271</v>
+        <v>1.7935970790688274</v>
       </c>
       <c r="U14" s="16">
         <f t="shared" si="15"/>
-        <v>1.4935970790688271</v>
+        <v>1.8935970790688275</v>
       </c>
       <c r="V14" s="16">
-        <f t="shared" ref="V14:Y14" si="16">U14+$O14</f>
-        <v>1.4935970790688271</v>
+        <f t="shared" ref="V14:X14" si="16">U14+$O14</f>
+        <v>1.9935970790688275</v>
       </c>
       <c r="W14" s="16">
         <f t="shared" si="16"/>
-        <v>1.4935970790688271</v>
+        <v>2.0935970790688274</v>
       </c>
       <c r="X14" s="16">
         <f t="shared" si="16"/>
-        <v>1.4935970790688271</v>
+        <v>2.1935970790688275</v>
       </c>
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
@@ -32734,7 +32512,7 @@
       </c>
       <c r="E15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32742,19 +32520,19 @@
       </c>
       <c r="G15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J15" s="13">
         <f>VLOOKUP(VLOOKUP($A15,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -32785,7 +32563,7 @@
         <v>1.2865935867004883</v>
       </c>
       <c r="V15" s="16">
-        <f t="shared" ref="V15:Y15" si="18">U15+$O15</f>
+        <f t="shared" ref="V15:X15" si="18">U15+$O15</f>
         <v>1.4865935867004882</v>
       </c>
       <c r="W15" s="16">
@@ -32826,7 +32604,7 @@
       </c>
       <c r="E16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32834,23 +32612,26 @@
       </c>
       <c r="G16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J16" s="13">
         <f>VLOOKUP(VLOOKUP($A16,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
+      <c r="O16">
+        <v>0.1</v>
+      </c>
       <c r="P16" t="s">
         <v>232</v>
       </c>
@@ -32859,31 +32640,31 @@
       </c>
       <c r="R16" s="16">
         <f t="shared" ref="R16" si="19">Q16+$O16</f>
-        <v>1.4468415717265699</v>
+        <v>1.54684157172657</v>
       </c>
       <c r="S16" s="16">
         <f t="shared" ref="S16" si="20">R16+$O16</f>
-        <v>1.4468415717265699</v>
+        <v>1.6468415717265701</v>
       </c>
       <c r="T16" s="16">
         <f t="shared" ref="T16" si="21">S16+$O16</f>
-        <v>1.4468415717265699</v>
+        <v>1.7468415717265702</v>
       </c>
       <c r="U16" s="16">
         <f t="shared" ref="U16" si="22">T16+$O16</f>
-        <v>1.4468415717265699</v>
+        <v>1.8468415717265703</v>
       </c>
       <c r="V16" s="16">
         <f t="shared" ref="V16" si="23">U16+$O16</f>
-        <v>1.4468415717265699</v>
+        <v>1.9468415717265704</v>
       </c>
       <c r="W16" s="16">
         <f t="shared" ref="W16" si="24">V16+$O16</f>
-        <v>1.4468415717265699</v>
+        <v>2.0468415717265702</v>
       </c>
       <c r="X16" s="16">
-        <f t="shared" ref="X16:Y16" si="25">W16+$O16</f>
-        <v>1.4468415717265699</v>
+        <f t="shared" ref="X16" si="25">W16+$O16</f>
+        <v>2.1468415717265703</v>
       </c>
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
@@ -32915,7 +32696,7 @@
       </c>
       <c r="E17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -32923,19 +32704,19 @@
       </c>
       <c r="G17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J17" s="13">
         <f>VLOOKUP(VLOOKUP($A17,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -32947,32 +32728,32 @@
         <v>3.1664804701843869</v>
       </c>
       <c r="R17" s="16">
-        <f t="shared" ref="R17:Y19" si="26">Q17+$O16</f>
-        <v>3.1664804701843869</v>
+        <f t="shared" ref="R17:X19" si="26">Q17+$O16</f>
+        <v>3.266480470184387</v>
       </c>
       <c r="S17" s="16">
         <f t="shared" si="26"/>
-        <v>3.1664804701843869</v>
+        <v>3.3664804701843871</v>
       </c>
       <c r="T17" s="16">
         <f t="shared" si="26"/>
-        <v>3.1664804701843869</v>
+        <v>3.4664804701843872</v>
       </c>
       <c r="U17" s="16">
         <f t="shared" si="26"/>
-        <v>3.1664804701843869</v>
+        <v>3.5664804701843873</v>
       </c>
       <c r="V17" s="16">
         <f t="shared" si="26"/>
-        <v>3.1664804701843869</v>
+        <v>3.6664804701843874</v>
       </c>
       <c r="W17" s="16">
         <f t="shared" si="26"/>
-        <v>3.1664804701843869</v>
+        <v>3.7664804701843875</v>
       </c>
       <c r="X17" s="16">
         <f t="shared" si="26"/>
-        <v>3.1664804701843869</v>
+        <v>3.8664804701843876</v>
       </c>
       <c r="Y17" s="13"/>
       <c r="Z17" s="13"/>
@@ -33004,7 +32785,7 @@
       </c>
       <c r="E18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33012,19 +32793,19 @@
       </c>
       <c r="G18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J18" s="13">
         <f>VLOOKUP(VLOOKUP($A18,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
@@ -33091,7 +32872,7 @@
       </c>
       <c r="E19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33099,19 +32880,19 @@
       </c>
       <c r="G19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J19" s="13">
         <f>VLOOKUP(VLOOKUP($A19,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
@@ -33178,7 +32959,7 @@
       </c>
       <c r="E20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33186,19 +32967,19 @@
       </c>
       <c r="G20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J20" s="13">
         <f>VLOOKUP(VLOOKUP($A20,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
@@ -33238,7 +33019,7 @@
       </c>
       <c r="E21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33246,19 +33027,19 @@
       </c>
       <c r="G21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J21" s="13">
         <f>VLOOKUP(VLOOKUP($A21,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
@@ -33298,7 +33079,7 @@
       </c>
       <c r="E22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33306,19 +33087,19 @@
       </c>
       <c r="G22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J22" s="13">
         <f>VLOOKUP(VLOOKUP($A22,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
@@ -33358,7 +33139,7 @@
       </c>
       <c r="E23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33366,19 +33147,19 @@
       </c>
       <c r="G23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J23" s="13">
         <f>VLOOKUP(VLOOKUP($A23,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
@@ -33418,7 +33199,7 @@
       </c>
       <c r="E24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33426,19 +33207,19 @@
       </c>
       <c r="G24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J24" s="13">
         <f>VLOOKUP(VLOOKUP($A24,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
@@ -33478,7 +33259,7 @@
       </c>
       <c r="E25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33486,19 +33267,19 @@
       </c>
       <c r="G25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J25" s="13">
         <f>VLOOKUP(VLOOKUP($A25,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
@@ -33538,7 +33319,7 @@
       </c>
       <c r="E26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33546,19 +33327,19 @@
       </c>
       <c r="G26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J26" s="13">
         <f>VLOOKUP(VLOOKUP($A26,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
@@ -33598,7 +33379,7 @@
       </c>
       <c r="E27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33606,19 +33387,19 @@
       </c>
       <c r="G27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J27" s="13">
         <f>VLOOKUP(VLOOKUP($A27,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
@@ -33658,7 +33439,7 @@
       </c>
       <c r="E28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18419376830713063</v>
+        <v>0.20465974256347846</v>
       </c>
       <c r="F28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33666,19 +33447,19 @@
       </c>
       <c r="G28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="H28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.1256285840991316</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="I28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.92096884153565306</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="J28" s="13">
         <f>VLOOKUP(VLOOKUP($A28,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.81863897025391386</v>
+        <v>1.2279584553808707</v>
       </c>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
@@ -33718,7 +33499,7 @@
       </c>
       <c r="E29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.35455122421838264</v>
+        <v>0.39394580468709184</v>
       </c>
       <c r="F29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33726,19 +33507,19 @@
       </c>
       <c r="G29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.2867019257790051</v>
+        <v>1.4036748281225508</v>
       </c>
       <c r="H29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.84670192577900516</v>
+        <v>0.92367482812255086</v>
       </c>
       <c r="I29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.33275612109191322</v>
+        <v>0.44367482812255093</v>
       </c>
       <c r="J29" s="13">
         <f>VLOOKUP(VLOOKUP($A29,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>-2.4216781251632735E-2</v>
+        <v>-3.6325171877449103E-2</v>
       </c>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
@@ -33778,7 +33559,7 @@
       </c>
       <c r="E30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.35455122421838264</v>
+        <v>0.39394580468709184</v>
       </c>
       <c r="F30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33786,19 +33567,19 @@
       </c>
       <c r="G30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.2867019257790051</v>
+        <v>1.4036748281225508</v>
       </c>
       <c r="H30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.84670192577900516</v>
+        <v>0.92367482812255086</v>
       </c>
       <c r="I30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.33275612109191322</v>
+        <v>0.44367482812255093</v>
       </c>
       <c r="J30" s="13">
         <f>VLOOKUP(VLOOKUP($A30,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>-2.4216781251632735E-2</v>
+        <v>-3.6325171877449103E-2</v>
       </c>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
@@ -33838,7 +33619,7 @@
       </c>
       <c r="E31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.35455122421838264</v>
+        <v>0.39394580468709184</v>
       </c>
       <c r="F31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33846,19 +33627,19 @@
       </c>
       <c r="G31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.2867019257790051</v>
+        <v>1.4036748281225508</v>
       </c>
       <c r="H31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.84670192577900516</v>
+        <v>0.92367482812255086</v>
       </c>
       <c r="I31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.33275612109191322</v>
+        <v>0.44367482812255093</v>
       </c>
       <c r="J31" s="13">
         <f>VLOOKUP(VLOOKUP($A31,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>-2.4216781251632735E-2</v>
+        <v>-3.6325171877449103E-2</v>
       </c>
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
@@ -33898,7 +33679,7 @@
       </c>
       <c r="E32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33906,19 +33687,19 @@
       </c>
       <c r="G32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J32" s="13">
         <f>VLOOKUP(VLOOKUP($A32,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
@@ -33958,7 +33739,7 @@
       </c>
       <c r="E33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -33966,19 +33747,19 @@
       </c>
       <c r="G33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J33" s="13">
         <f>VLOOKUP(VLOOKUP($A33,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
@@ -34018,7 +33799,7 @@
       </c>
       <c r="E34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34026,19 +33807,19 @@
       </c>
       <c r="G34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J34" s="13">
         <f>VLOOKUP(VLOOKUP($A34,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
@@ -34078,7 +33859,7 @@
       </c>
       <c r="E35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34086,19 +33867,19 @@
       </c>
       <c r="G35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J35" s="13">
         <f>VLOOKUP(VLOOKUP($A35,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
@@ -34138,7 +33919,7 @@
       </c>
       <c r="E36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34146,19 +33927,19 @@
       </c>
       <c r="G36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J36" s="13">
         <f>VLOOKUP(VLOOKUP($A36,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
@@ -34198,7 +33979,7 @@
       </c>
       <c r="E37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34206,19 +33987,19 @@
       </c>
       <c r="G37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J37" s="13">
         <f>VLOOKUP(VLOOKUP($A37,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
@@ -34258,7 +34039,7 @@
       </c>
       <c r="E38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34266,19 +34047,19 @@
       </c>
       <c r="G38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J38" s="13">
         <f>VLOOKUP(VLOOKUP($A38,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
@@ -34318,7 +34099,7 @@
       </c>
       <c r="E39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34326,19 +34107,19 @@
       </c>
       <c r="G39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J39" s="13">
         <f>VLOOKUP(VLOOKUP($A39,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K39" s="13"/>
       <c r="L39" s="13"/>
@@ -34378,7 +34159,7 @@
       </c>
       <c r="E40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34386,19 +34167,19 @@
       </c>
       <c r="G40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J40" s="13">
         <f>VLOOKUP(VLOOKUP($A40,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K40" s="13"/>
       <c r="L40" s="13"/>
@@ -34438,7 +34219,7 @@
       </c>
       <c r="E41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34446,19 +34227,19 @@
       </c>
       <c r="G41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J41" s="13">
         <f>VLOOKUP(VLOOKUP($A41,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
@@ -34498,7 +34279,7 @@
       </c>
       <c r="E42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34506,19 +34287,19 @@
       </c>
       <c r="G42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J42" s="13">
         <f>VLOOKUP(VLOOKUP($A42,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K42" s="13"/>
       <c r="L42" s="13"/>
@@ -34558,7 +34339,7 @@
       </c>
       <c r="E43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34566,19 +34347,19 @@
       </c>
       <c r="G43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J43" s="13">
         <f>VLOOKUP(VLOOKUP($A43,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K43" s="13"/>
       <c r="L43" s="13"/>
@@ -34618,7 +34399,7 @@
       </c>
       <c r="E44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34626,19 +34407,19 @@
       </c>
       <c r="G44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J44" s="13">
         <f>VLOOKUP(VLOOKUP($A44,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K44" s="13"/>
       <c r="L44" s="13"/>
@@ -34678,7 +34459,7 @@
       </c>
       <c r="E45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34686,19 +34467,19 @@
       </c>
       <c r="G45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J45" s="13">
         <f>VLOOKUP(VLOOKUP($A45,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K45" s="13"/>
       <c r="L45" s="13"/>
@@ -34738,7 +34519,7 @@
       </c>
       <c r="E46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34746,19 +34527,19 @@
       </c>
       <c r="G46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J46" s="13">
         <f>VLOOKUP(VLOOKUP($A46,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K46" s="13"/>
       <c r="L46" s="13"/>
@@ -34798,7 +34579,7 @@
       </c>
       <c r="E47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34806,19 +34587,19 @@
       </c>
       <c r="G47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J47" s="13">
         <f>VLOOKUP(VLOOKUP($A47,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K47" s="13"/>
       <c r="L47" s="13"/>
@@ -34858,7 +34639,7 @@
       </c>
       <c r="E48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34866,19 +34647,19 @@
       </c>
       <c r="G48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J48" s="13">
         <f>VLOOKUP(VLOOKUP($A48,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
@@ -34918,7 +34699,7 @@
       </c>
       <c r="E49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15820911233515481</v>
+        <v>0.17578790259461644</v>
       </c>
       <c r="F49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -34926,19 +34707,19 @@
       </c>
       <c r="G49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4068334642703904</v>
+        <v>1.5347274155676984</v>
       </c>
       <c r="H49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6268334642703903</v>
+        <v>1.7747274155676984</v>
       </c>
       <c r="I49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5110455616757739</v>
+        <v>2.0147274155676982</v>
       </c>
       <c r="J49" s="13">
         <f>VLOOKUP(VLOOKUP($A49,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5031516103784657</v>
+        <v>2.2547274155676984</v>
       </c>
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
@@ -35030,7 +34811,7 @@
       </c>
       <c r="E51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.20603917268586067</v>
+        <v>0.22893241409540074</v>
       </c>
       <c r="F51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -35038,19 +34819,19 @@
       </c>
       <c r="G51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.2591282775247041</v>
+        <v>1.3735944845724044</v>
       </c>
       <c r="H51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.2591282775247041</v>
+        <v>1.3735944845724044</v>
       </c>
       <c r="I51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.0301958634293034</v>
+        <v>1.3735944845724044</v>
       </c>
       <c r="J51" s="13">
         <f>VLOOKUP(VLOOKUP($A51,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.91572965638160297</v>
+        <v>1.3735944845724044</v>
       </c>
       <c r="K51" s="13"/>
       <c r="L51" s="13"/>
@@ -35090,7 +34871,7 @@
       </c>
       <c r="E52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.21179989820782757</v>
+        <v>0.23533322023091952</v>
       </c>
       <c r="F52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -35098,19 +34879,19 @@
       </c>
       <c r="G52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.2943327112700573</v>
+        <v>1.4119993213855171</v>
       </c>
       <c r="H52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.2943327112700573</v>
+        <v>1.4119993213855171</v>
       </c>
       <c r="I52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.0589994910391378</v>
+        <v>1.4119993213855171</v>
       </c>
       <c r="J52" s="13">
         <f>VLOOKUP(VLOOKUP($A52,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.94133288092367806</v>
+        <v>1.4119993213855171</v>
       </c>
       <c r="K52" s="13"/>
       <c r="L52" s="13"/>
@@ -35150,7 +34931,7 @@
       </c>
       <c r="E53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18622589858760141</v>
+        <v>0.20691766509733489</v>
       </c>
       <c r="F53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -35158,19 +34939,19 @@
       </c>
       <c r="G53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.138047158035342</v>
+        <v>1.2415059905840091</v>
       </c>
       <c r="H53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.138047158035342</v>
+        <v>1.2415059905840091</v>
       </c>
       <c r="I53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.93112949293800695</v>
+        <v>1.2415059905840091</v>
       </c>
       <c r="J53" s="13">
         <f>VLOOKUP(VLOOKUP($A53,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.82767066038933956</v>
+        <v>1.2415059905840091</v>
       </c>
       <c r="K53" s="13"/>
       <c r="L53" s="13"/>
@@ -35210,27 +34991,27 @@
       </c>
       <c r="E54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.26884747423238892</v>
+        <v>0.33871941581376547</v>
       </c>
       <c r="F54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.64295678697571</v>
+        <v>1.9729567869757103</v>
       </c>
       <c r="G54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.64295678697571</v>
+        <v>2.2723164948825927</v>
       </c>
       <c r="H54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.64295678697571</v>
+        <v>2.3923164948825928</v>
       </c>
       <c r="I54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3442373711619444</v>
+        <v>2.5123164948825929</v>
       </c>
       <c r="J54" s="13">
         <f>VLOOKUP(VLOOKUP($A54,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.1948776632550617</v>
+        <v>2.632316494882593</v>
       </c>
       <c r="K54" s="13"/>
       <c r="L54" s="13"/>
@@ -35270,7 +35051,7 @@
       </c>
       <c r="E55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.18622589858760141</v>
+        <v>0.20691766509733489</v>
       </c>
       <c r="F55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -35278,19 +35059,19 @@
       </c>
       <c r="G55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.138047158035342</v>
+        <v>1.2415059905840091</v>
       </c>
       <c r="H55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.138047158035342</v>
+        <v>1.2415059905840091</v>
       </c>
       <c r="I55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.93112949293800695</v>
+        <v>1.2415059905840091</v>
       </c>
       <c r="J55" s="13">
         <f>VLOOKUP(VLOOKUP($A55,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.82767066038933956</v>
+        <v>1.2415059905840091</v>
       </c>
       <c r="K55" s="13"/>
       <c r="L55" s="13"/>
@@ -35330,27 +35111,27 @@
       </c>
       <c r="E56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.26884747423238892</v>
+        <v>0.33871941581376547</v>
       </c>
       <c r="F56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.64295678697571</v>
+        <v>1.9729567869757103</v>
       </c>
       <c r="G56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.64295678697571</v>
+        <v>2.2723164948825927</v>
       </c>
       <c r="H56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.64295678697571</v>
+        <v>2.3923164948825928</v>
       </c>
       <c r="I56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.3442373711619444</v>
+        <v>2.5123164948825929</v>
       </c>
       <c r="J56" s="13">
         <f>VLOOKUP(VLOOKUP($A56,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.1948776632550617</v>
+        <v>2.632316494882593</v>
       </c>
       <c r="K56" s="13"/>
       <c r="L56" s="13"/>
@@ -35390,27 +35171,27 @@
       </c>
       <c r="E57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.26043148291078261</v>
+        <v>0.32936831434531405</v>
       </c>
       <c r="F57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>1.5915257288992271</v>
+        <v>1.9215257288992273</v>
       </c>
       <c r="G57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.5915257288992271</v>
+        <v>2.2162098860718844</v>
       </c>
       <c r="H57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.5915257288992271</v>
+        <v>2.3362098860718845</v>
       </c>
       <c r="I57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.302157414553913</v>
+        <v>2.4562098860718842</v>
       </c>
       <c r="J57" s="13">
         <f>VLOOKUP(VLOOKUP($A57,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.1574732573812561</v>
+        <v>2.5762098860718843</v>
       </c>
       <c r="K57" s="13"/>
       <c r="L57" s="13"/>
@@ -35450,27 +35231,27 @@
       </c>
       <c r="E58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.56996648463318966</v>
+        <v>0.67329609403687751</v>
       </c>
       <c r="F58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
-        <v>3.4831285172028261</v>
+        <v>3.8131285172028262</v>
       </c>
       <c r="G58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>3.4831285172028261</v>
+        <v>4.2797765642212644</v>
       </c>
       <c r="H58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>3.4831285172028261</v>
+        <v>4.3997765642212645</v>
       </c>
       <c r="I58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>2.8498324231659482</v>
+        <v>4.5197765642212646</v>
       </c>
       <c r="J58" s="13">
         <f>VLOOKUP(VLOOKUP($A58,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>2.5331843761475099</v>
+        <v>4.6397765642212647</v>
       </c>
       <c r="K58" s="13"/>
       <c r="L58" s="13"/>
@@ -35510,7 +35291,7 @@
       </c>
       <c r="E59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.15958684560608793</v>
+        <v>0.17731871734009769</v>
       </c>
       <c r="F59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -35518,19 +35299,19 @@
       </c>
       <c r="G59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.4152529453705371</v>
+        <v>1.543912304040586</v>
       </c>
       <c r="H59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.6352529453705371</v>
+        <v>1.7839123040405858</v>
       </c>
       <c r="I59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5179342280304393</v>
+        <v>2.0239123040405858</v>
       </c>
       <c r="J59" s="13">
         <f>VLOOKUP(VLOOKUP($A59,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.5092748693603906</v>
+        <v>2.2639123040405855</v>
       </c>
       <c r="K59" s="13"/>
       <c r="L59" s="13"/>
@@ -35570,7 +35351,7 @@
       </c>
       <c r="E60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>6.1818662961653476E-2</v>
+        <v>6.8687403290726076E-2</v>
       </c>
       <c r="F60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -35578,19 +35359,19 @@
       </c>
       <c r="G60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>0.37778071809899344</v>
+        <v>0.41212441974435648</v>
       </c>
       <c r="H60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>0.37778071809899344</v>
+        <v>0.41212441974435648</v>
       </c>
       <c r="I60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>0.30909331480826735</v>
+        <v>0.41212441974435648</v>
       </c>
       <c r="J60" s="13">
         <f>VLOOKUP(VLOOKUP($A60,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>0.2747496131629043</v>
+        <v>0.41212441974435648</v>
       </c>
       <c r="K60" s="13"/>
       <c r="L60" s="13"/>
@@ -35630,7 +35411,7 @@
       </c>
       <c r="E61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.31414350042015632</v>
+        <v>0.34904833380017369</v>
       </c>
       <c r="F61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -35638,19 +35419,19 @@
       </c>
       <c r="G61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.9197658359009553</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="H61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.9197658359009553</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="I61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5707175021007815</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="J61" s="13">
         <f>VLOOKUP(VLOOKUP($A61,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.3961933352006948</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="K61" s="13"/>
       <c r="L61" s="13"/>
@@ -35690,7 +35471,7 @@
       </c>
       <c r="E62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.31414350042015632</v>
+        <v>0.34904833380017369</v>
       </c>
       <c r="F62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -35698,19 +35479,19 @@
       </c>
       <c r="G62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.9197658359009553</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="H62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.9197658359009553</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="I62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5707175021007815</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="J62" s="13">
         <f>VLOOKUP(VLOOKUP($A62,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.3961933352006948</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="K62" s="13"/>
       <c r="L62" s="13"/>
@@ -35750,7 +35531,7 @@
       </c>
       <c r="E63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:S$7),)*E$3</f>
-        <v>0.31414350042015632</v>
+        <v>0.34904833380017369</v>
       </c>
       <c r="F63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:T$7),)*F$3</f>
@@ -35758,19 +35539,19 @@
       </c>
       <c r="G63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:U$7),)*G$3</f>
-        <v>1.9197658359009553</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="H63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:V$7),)*H$3</f>
-        <v>1.9197658359009553</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="I63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:W$7),)*I$3</f>
-        <v>1.5707175021007815</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="J63" s="13">
         <f>VLOOKUP(VLOOKUP($A63,$AC$7:$AD$62,2,0),$P$8:$X$19,COLUMNS($P$7:X$7),)*J$3</f>
-        <v>1.3961933352006948</v>
+        <v>2.094290002801042</v>
       </c>
       <c r="K63" s="13"/>
       <c r="L63" s="13"/>
@@ -35964,262 +35745,262 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C55:C56 C64:E70 C59 C33:C50 C30:C31 C9:C28 C62:C63 H64:H70 J64:M70 K8:M63 S8:U8 S18:AB18 Y8:AB8 Y9:Z17 AB9:AB17 S17:X18 S10:X15 S20:AB70 Y19:AB19">
-    <cfRule type="cellIs" dxfId="133" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="65" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:U8 S18:AB18 Y8:AB8 Y9:Z17 AB9:AB17 S20:AB70 Y19:AB19">
-    <cfRule type="cellIs" dxfId="132" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="64" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64:I70">
-    <cfRule type="cellIs" dxfId="131" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="63" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G64:G70">
-    <cfRule type="cellIs" dxfId="130" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="62" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1">
-    <cfRule type="cellIs" dxfId="129" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="52" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:J63">
-    <cfRule type="cellIs" dxfId="128" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="51" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:N1 R1 P1">
-    <cfRule type="cellIs" dxfId="127" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="57" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1">
-    <cfRule type="cellIs" dxfId="126" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="56" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1">
-    <cfRule type="cellIs" dxfId="125" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="55" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1 Q1">
-    <cfRule type="cellIs" dxfId="124" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="54" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1">
-    <cfRule type="cellIs" dxfId="123" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="53" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="122" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="36" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="121" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="35" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:E8 G8:J8">
-    <cfRule type="cellIs" dxfId="120" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="43" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="119" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="42" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="118" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="41" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8 I8">
-    <cfRule type="cellIs" dxfId="117" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="40" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="116" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="39" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="115" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="38" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="114" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="37" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C53">
-    <cfRule type="cellIs" dxfId="113" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="34" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="112" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="33" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="cellIs" dxfId="111" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="32" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="110" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="31" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="109" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="30" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55:E56 D62:E63 D58:E59 D33:E50 D30:E31 D9:E28 G9:J28 G30:J31 G33:J50 G58:J59 G62:J63 G55:J56">
-    <cfRule type="cellIs" dxfId="108" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="29" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:E29 G29:J29">
-    <cfRule type="cellIs" dxfId="107" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="28" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:E32 G32:J32">
-    <cfRule type="cellIs" dxfId="106" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="27" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:E51 G51:J51">
-    <cfRule type="cellIs" dxfId="105" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="26" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:E53 G52:J53">
-    <cfRule type="cellIs" dxfId="104" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="25" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54:E54 G54:J54">
-    <cfRule type="cellIs" dxfId="103" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="24" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:E57 G57:J57">
-    <cfRule type="cellIs" dxfId="102" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="23" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60:E60 G60:J60">
-    <cfRule type="cellIs" dxfId="101" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="22" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61:E61 G61:J61">
-    <cfRule type="cellIs" dxfId="100" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="21" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F64:F70">
-    <cfRule type="cellIs" dxfId="99" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="20" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="98" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="19" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="97" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="18" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55:F56 F62:F63 F58:F59 F33:F50 F30:F31 F9:F28">
-    <cfRule type="cellIs" dxfId="96" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="17" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29">
-    <cfRule type="cellIs" dxfId="95" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="16" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="94" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="15" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51">
-    <cfRule type="cellIs" dxfId="93" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="14" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:F53">
-    <cfRule type="cellIs" dxfId="92" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="13" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="cellIs" dxfId="91" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="12" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57">
-    <cfRule type="cellIs" dxfId="90" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60">
-    <cfRule type="cellIs" dxfId="89" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61">
-    <cfRule type="cellIs" dxfId="88" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V8:X8">
-    <cfRule type="cellIs" dxfId="87" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V8:X8">
-    <cfRule type="cellIs" dxfId="86" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S16:X16">
-    <cfRule type="cellIs" dxfId="85" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="cellIs" dxfId="84" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19:X19">
-    <cfRule type="cellIs" dxfId="83" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S19:X19">
-    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41311,12 +41092,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8:C63 D7:L63 C10:L70 R8:AA70">
-    <cfRule type="cellIs" dxfId="81" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="12" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:AA70">
-    <cfRule type="cellIs" dxfId="80" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42400,42 +42181,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:K7 B8:K17 Q8:Z17 Q19:Z21 B19:K21">
-    <cfRule type="cellIs" dxfId="79" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="19" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z17">
-    <cfRule type="cellIs" dxfId="78" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z17">
-    <cfRule type="cellIs" dxfId="77" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z17">
-    <cfRule type="cellIs" dxfId="76" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:K18 Q18:Z18">
-    <cfRule type="cellIs" dxfId="75" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q18:Z18">
-    <cfRule type="cellIs" dxfId="74" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18:Z18">
-    <cfRule type="cellIs" dxfId="73" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R18:Z18">
-    <cfRule type="cellIs" dxfId="72" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43316,62 +43097,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:K7 Q8:Z16 B8:K16">
-    <cfRule type="cellIs" dxfId="71" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="30" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z16">
-    <cfRule type="cellIs" dxfId="70" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="24" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="69" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="23" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="68" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="22" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="67" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="21" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z16">
-    <cfRule type="cellIs" dxfId="66" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="20" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17 B17:K17">
-    <cfRule type="cellIs" dxfId="65" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17">
-    <cfRule type="cellIs" dxfId="64" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="63" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="62" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17:Z17">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44216,57 +43997,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C7:K7 Q8:Z13 B8:K16">
-    <cfRule type="cellIs" dxfId="59" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:Z13">
-    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="10" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="9" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8:Z13">
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:Z16">
-    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="5" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14:Z16">
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:K17">
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17">
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17:Z17">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>"eps"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>